<commit_message>
Fix typo in investment cost category.
</commit_message>
<xml_diff>
--- a/pycba/examples/lietavska_lucka/inputs.xlsx
+++ b/pycba/examples/lietavska_lucka/inputs.xlsx
@@ -59,7 +59,7 @@
     <t xml:space="preserve">walls and stabilisation</t>
   </si>
   <si>
-    <t xml:space="preserve">noise barriers and other enviroment protection measures</t>
+    <t xml:space="preserve">noise barriers and other environment protection measures</t>
   </si>
   <si>
     <t xml:space="preserve">information system – constructions</t>
@@ -593,7 +593,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Tweak Lietavska Lucka example input.
</commit_message>
<xml_diff>
--- a/pycba/examples/lietavska_lucka/inputs.xlsx
+++ b/pycba/examples/lietavska_lucka/inputs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="capex" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
     <sheet name="velocities_1" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">road_parameters!$A$1:$X$72</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">road_parameters!$A$1:$X$74</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="97">
   <si>
     <t xml:space="preserve">item</t>
   </si>
@@ -209,10 +209,13 @@
     <t xml:space="preserve">(Slnečné Skaly - Lietavská Lúčka) intravilan Porubka – mosty</t>
   </si>
   <si>
-    <t xml:space="preserve">(Slnečné Skaly - Lietavská Lúčka) kon. Intravilan Porubka – kriz. III/2104</t>
+    <t xml:space="preserve">(Slnečné Skaly - Lietavská Lúčka) kon. Intravilan Porubka – kriz. III/2104 – cesty</t>
   </si>
   <si>
     <t xml:space="preserve">064-056</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Slnečné Skaly - Lietavská Lúčka) kon. Intravilan Porubka – kriz. III/2104 – mosty</t>
   </si>
   <si>
     <t xml:space="preserve">(Lietavská Lúčka - Križovatka Solinky)  kriz. III/2104 – zac. Intavilan LL</t>
@@ -249,6 +252,9 @@
   </si>
   <si>
     <t xml:space="preserve">(Križovatka LL - Križovatka Solinky) I/65b x D1 – Solinky – mosty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Slnečné Skaly - Lietavská Lúčka) kon. Intravilan Porubka – kriz. III/2104</t>
   </si>
   <si>
     <t xml:space="preserve">Slnečné Skaly - Križovatka LL – cesty</t>
@@ -592,7 +598,7 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -869,16 +875,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y72"/>
+  <dimension ref="A1:Y74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q2" activeCellId="0" sqref="Q2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N20" activeCellId="0" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="14.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="61.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="72.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="8.86"/>
@@ -1247,7 +1253,8 @@
         <v>0</v>
       </c>
       <c r="F7" s="4" t="n">
-        <v>0.3</v>
+        <f aca="false">0.3-0.007</f>
+        <v>0.293</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>8</v>
@@ -1283,34 +1290,33 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
-        <v>201</v>
+        <v>107</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F8" s="4" t="n">
-        <v>0.5</v>
+        <v>0.007</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>44</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K8" s="6" t="n">
-        <f aca="false">FALSE()</f>
+        <v>45</v>
+      </c>
+      <c r="K8" s="6" t="b">
         <v>0</v>
       </c>
       <c r="L8" s="2" t="s">
@@ -1326,18 +1332,18 @@
         <v>47</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>2</v>
@@ -1349,8 +1355,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="4" t="n">
-        <f aca="false">3.9-0.04</f>
-        <v>3.86</v>
+        <v>0.5</v>
       </c>
       <c r="G9" s="2" t="n">
         <v>9</v>
@@ -1366,7 +1371,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>43</v>
@@ -1378,30 +1383,31 @@
         <v>47</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F10" s="4" t="n">
-        <v>0.04</v>
+        <f aca="false">3.9-0.033</f>
+        <v>3.867</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>9</v>
@@ -1410,7 +1416,7 @@
         <v>44</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="K10" s="6" t="n">
         <f aca="false">FALSE()</f>
@@ -1429,83 +1435,82 @@
         <v>47</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
-        <v>301</v>
+        <v>203</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F11" s="4" t="n">
-        <f aca="false">3.5 - 1.582</f>
-        <v>1.918</v>
+        <v>0.033</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>22.5</v>
+        <v>9</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>44</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="K11" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>43</v>
       </c>
       <c r="N11" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F12" s="4" t="n">
-        <f aca="false">1.582</f>
-        <v>1.582</v>
+        <f aca="false">3.5 - 1.582</f>
+        <v>1.918</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>22.5</v>
@@ -1514,7 +1519,7 @@
         <v>44</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K12" s="6" t="n">
         <f aca="false">FALSE()</f>
@@ -1530,97 +1535,95 @@
         <v>4</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
+        <v>302</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4" t="n">
+        <f aca="false">1.582</f>
+        <v>1.582</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K13" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N13" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
         <v>101</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="C14" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="E14" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="4" t="n">
+      <c r="F14" s="4" t="n">
         <f aca="false">1.5-0.003-0.56</f>
         <v>0.937</v>
       </c>
-      <c r="G13" s="2" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K13" s="6" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N13" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="n">
-        <v>102</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F14" s="4" t="n">
-        <v>0.003</v>
-      </c>
       <c r="G14" s="2" t="n">
         <v>7.5</v>
       </c>
-      <c r="H14" s="2" t="n">
-        <v>22.5</v>
-      </c>
       <c r="I14" s="2" t="s">
         <v>44</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="K14" s="6" t="n">
         <f aca="false">TRUE()</f>
@@ -1647,31 +1650,34 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E15" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F15" s="2" t="n">
-        <v>0.56</v>
+      <c r="F15" s="4" t="n">
+        <v>0.003</v>
       </c>
       <c r="G15" s="2" t="n">
         <v>7.5</v>
       </c>
+      <c r="H15" s="2" t="n">
+        <v>22.5</v>
+      </c>
       <c r="I15" s="2" t="s">
         <v>44</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="K15" s="6" t="n">
         <f aca="false">TRUE()</f>
@@ -1693,15 +1699,15 @@
         <v>48</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>1</v>
@@ -1712,12 +1718,11 @@
       <c r="E16" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F16" s="4" t="n">
-        <f aca="false">0.6-0.0293</f>
-        <v>0.5707</v>
+      <c r="F16" s="2" t="n">
+        <v>0.56</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>44</v>
@@ -1730,7 +1735,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>43</v>
@@ -1745,33 +1750,31 @@
         <v>48</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F17" s="4" t="n">
-        <v>0.0293</v>
+        <f aca="false">0.6-0.0293</f>
+        <v>0.5707</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>8</v>
-      </c>
-      <c r="H17" s="2" t="n">
-        <v>234.4</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>44</v>
@@ -1804,25 +1807,28 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E18" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F18" s="4" t="n">
-        <v>0.3</v>
+        <v>0.0293</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>8</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>234.4</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>44</v>
@@ -1835,7 +1841,7 @@
         <v>1</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>43</v>
@@ -1850,18 +1856,18 @@
         <v>48</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
-        <v>201</v>
+        <v>106</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>43</v>
@@ -1870,16 +1876,17 @@
         <v>1</v>
       </c>
       <c r="F19" s="4" t="n">
-        <v>0.5</v>
+        <f aca="false">0.3-0.007</f>
+        <v>0.293</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>44</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="K19" s="6" t="n">
         <f aca="false">TRUE()</f>
@@ -1898,47 +1905,45 @@
         <v>47</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
-        <v>202</v>
+        <v>107</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E20" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F20" s="4" t="n">
-        <f aca="false">3.9-0.04</f>
-        <v>3.86</v>
+        <v>0.007</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>44</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K20" s="6" t="n">
-        <f aca="false">TRUE()</f>
+        <v>45</v>
+      </c>
+      <c r="K20" s="6" t="b">
         <v>1</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>43</v>
@@ -1950,30 +1955,30 @@
         <v>47</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>1</v>
       </c>
       <c r="F21" s="4" t="n">
-        <v>0.04</v>
+        <v>0.5</v>
       </c>
       <c r="G21" s="2" t="n">
         <v>9</v>
@@ -1982,14 +1987,14 @@
         <v>44</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="K21" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>43</v>
@@ -2001,21 +2006,21 @@
         <v>47</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
-        <v>301</v>
+        <v>202</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>43</v>
@@ -2024,121 +2029,120 @@
         <v>1</v>
       </c>
       <c r="F22" s="4" t="n">
+        <f aca="false">3.9-0.033</f>
+        <v>3.867</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K22" s="6" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N22" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="n">
+        <v>203</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" s="4" t="n">
+        <v>0.033</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K23" s="6" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N23" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="n">
+        <v>301</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" s="4" t="n">
         <f aca="false">3.5 - 1.582</f>
         <v>1.918</v>
       </c>
-      <c r="G22" s="2" t="n">
+      <c r="G24" s="2" t="n">
         <v>22.5</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="K22" s="6" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N22" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="P22" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="n">
-        <v>302</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F23" s="4" t="n">
-        <f aca="false">1.582</f>
-        <v>1.582</v>
-      </c>
-      <c r="G23" s="2" t="n">
-        <v>22.5</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="K23" s="6" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N23" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="n">
-        <v>401</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F24" s="4" t="n">
-        <f aca="false">3.8-0.958</f>
-        <v>2.842</v>
-      </c>
-      <c r="G24" s="2" t="n">
-        <v>10.5</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>44</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K24" s="6" t="n">
         <f aca="false">FALSE()</f>
@@ -2151,27 +2155,27 @@
         <v>43</v>
       </c>
       <c r="N24" s="2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
-        <v>402</v>
+        <v>302</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>51</v>
@@ -2180,16 +2184,17 @@
         <v>1</v>
       </c>
       <c r="F25" s="4" t="n">
-        <v>0.958</v>
+        <f aca="false">1.582</f>
+        <v>1.582</v>
       </c>
       <c r="G25" s="2" t="n">
-        <v>10.5</v>
+        <v>22.5</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>44</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K25" s="6" t="n">
         <f aca="false">FALSE()</f>
@@ -2202,28 +2207,123 @@
         <v>43</v>
       </c>
       <c r="N25" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="n">
+        <v>401</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" s="4" t="n">
+        <f aca="false">3.8-0.958</f>
+        <v>2.842</v>
+      </c>
+      <c r="G26" s="2" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K26" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N26" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="O25" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="7"/>
-      <c r="D26" s="2"/>
-      <c r="K26" s="6"/>
+      <c r="O26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="2"/>
-      <c r="K27" s="6"/>
+      <c r="A27" s="2" t="n">
+        <v>402</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" s="4" t="n">
+        <v>0.958</v>
+      </c>
+      <c r="G27" s="2" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K27" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N27" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="7"/>
       <c r="D28" s="2"/>
       <c r="K28" s="6"/>
     </row>
@@ -2331,40 +2431,40 @@
       <c r="D54" s="2"/>
       <c r="K54" s="6"/>
     </row>
-    <row r="55" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
       <c r="K55" s="6"/>
-      <c r="L55" s="2"/>
-      <c r="M55" s="2"/>
-      <c r="N55" s="2"/>
-      <c r="O55" s="2"/>
-      <c r="P55" s="2"/>
-      <c r="Q55" s="2"/>
-      <c r="R55" s="2"/>
-      <c r="S55" s="2"/>
-      <c r="T55" s="2"/>
-      <c r="U55" s="2"/>
-      <c r="V55" s="2"/>
-      <c r="W55" s="2"/>
-      <c r="X55" s="2"/>
-      <c r="Y55" s="2"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D56" s="2"/>
       <c r="K56" s="6"/>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
       <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
       <c r="K57" s="6"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+      <c r="O57" s="2"/>
+      <c r="P57" s="2"/>
+      <c r="Q57" s="2"/>
+      <c r="R57" s="2"/>
+      <c r="S57" s="2"/>
+      <c r="T57" s="2"/>
+      <c r="U57" s="2"/>
+      <c r="V57" s="2"/>
+      <c r="W57" s="2"/>
+      <c r="X57" s="2"/>
+      <c r="Y57" s="2"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D58" s="2"/>
@@ -2426,8 +2526,16 @@
       <c r="D72" s="2"/>
       <c r="K72" s="6"/>
     </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D73" s="2"/>
+      <c r="K73" s="6"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D74" s="2"/>
+      <c r="K74" s="6"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:X72"/>
+  <autoFilter ref="A1:X74"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2459,13 +2567,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2473,10 +2581,10 @@
         <v>49</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2484,10 +2592,10 @@
         <v>54</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2495,10 +2603,10 @@
         <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2506,51 +2614,51 @@
         <v>60</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2582,22 +2690,22 @@
         <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2605,7 +2713,7 @@
         <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C2" s="8" t="n">
         <v>1E-008</v>
@@ -2623,10 +2731,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C3" s="8" t="n">
         <v>1E-008</v>
@@ -2677,7 +2785,7 @@
         <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D1" s="10" t="n">
         <v>2022</v>
@@ -2775,7 +2883,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -2867,7 +2975,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -2959,7 +3067,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -3051,7 +3159,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -3143,7 +3251,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -3235,7 +3343,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -3327,7 +3435,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -3419,7 +3527,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -3511,7 +3619,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -3603,7 +3711,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -3695,7 +3803,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -3787,7 +3895,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -3879,7 +3987,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -3971,7 +4079,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -4063,7 +4171,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -4186,7 +4294,7 @@
         <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D1" s="10" t="n">
         <v>2022</v>
@@ -4284,7 +4392,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G2" s="10" t="n">
         <v>2779.91803278689</v>
@@ -4378,7 +4486,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G3" s="10" t="n">
         <v>5559.83606557377</v>
@@ -4472,7 +4580,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G4" s="10" t="n">
         <v>7413.11475409836</v>
@@ -4566,7 +4674,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G5" s="10" t="n">
         <v>8339.75409836066</v>
@@ -4660,7 +4768,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G6" s="10" t="n">
         <v>179.877049180328</v>
@@ -4754,7 +4862,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G7" s="10" t="n">
         <v>359.754098360656</v>
@@ -4848,7 +4956,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G8" s="10" t="n">
         <v>479.672131147541</v>
@@ -4942,7 +5050,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G9" s="10" t="n">
         <v>539.631147540984</v>
@@ -5036,7 +5144,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E10" s="11"/>
       <c r="G10" s="10" t="n">
@@ -5131,7 +5239,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E11" s="11"/>
       <c r="G11" s="10" t="n">
@@ -5226,7 +5334,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E12" s="11"/>
       <c r="G12" s="10" t="n">
@@ -5321,7 +5429,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G13" s="10" t="n">
         <v>236.739130434783</v>
@@ -5415,7 +5523,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E14" s="11"/>
       <c r="G14" s="10" t="n">
@@ -5510,7 +5618,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E15" s="11"/>
       <c r="G15" s="10" t="n">
@@ -5605,7 +5713,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E16" s="11"/>
       <c r="G16" s="10" t="n">
@@ -5700,7 +5808,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G17" s="10" t="n">
         <v>520.826086956522</v>
@@ -5794,7 +5902,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G18" s="10" t="n">
         <v>47.3478260869565</v>
@@ -5888,7 +5996,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G19" s="10" t="n">
         <v>94.6956521739131</v>
@@ -5982,7 +6090,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G20" s="10" t="n">
         <v>126.260869565217</v>
@@ -6076,7 +6184,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G21" s="10" t="n">
         <v>142.04347826087</v>
@@ -7318,7 +7426,7 @@
         <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D1" s="10" t="n">
         <v>2022</v>
@@ -7416,7 +7524,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -7508,7 +7616,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -7600,7 +7708,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -7692,7 +7800,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -7784,7 +7892,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -7876,7 +7984,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -7968,7 +8076,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -8060,7 +8168,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -8152,7 +8260,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -8244,7 +8352,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -8336,7 +8444,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -8428,7 +8536,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -8520,7 +8628,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -8612,7 +8720,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -8704,7 +8812,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -12900,7 +13008,7 @@
         <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D1" s="10" t="n">
         <v>2022</v>
@@ -12998,7 +13106,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -13090,7 +13198,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -13182,7 +13290,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -13274,7 +13382,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -13366,7 +13474,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -13458,7 +13566,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -13550,7 +13658,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -13642,7 +13750,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -13734,7 +13842,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -13826,7 +13934,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -13918,7 +14026,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -14010,7 +14118,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -14102,7 +14210,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -14194,7 +14302,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -14286,7 +14394,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -14378,7 +14486,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -14470,7 +14578,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -14562,7 +14670,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -14654,7 +14762,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
@@ -14746,7 +14854,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>

</xml_diff>